<commit_message>
chore: update epidemiological weeks to include 2024
</commit_message>
<xml_diff>
--- a/data/bronze/dengue_prudente_weekly.xlsx
+++ b/data/bronze/dengue_prudente_weekly.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryann\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryann\Documents\Projetos RStudio\dengue-project\data\bronze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78072A6E-F44B-422E-A526-EF28E6CD47FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28E787D-C558-4F74-8444-F2C8DF5F73C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="100">
   <si>
     <t>Região|UF|Município</t>
   </si>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,6 +706,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -723,6 +726,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -740,6 +746,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -757,6 +766,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -774,6 +786,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -791,6 +806,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -808,6 +826,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -825,6 +846,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -842,6 +866,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -859,6 +886,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -876,6 +906,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -893,6 +926,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -910,6 +946,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -927,6 +966,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -944,6 +986,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
@@ -960,7 +1005,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -977,7 +1025,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
@@ -994,7 +1045,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
@@ -1011,7 +1065,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +1085,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
@@ -1045,7 +1105,10 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
@@ -1062,7 +1125,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
@@ -1079,7 +1145,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1096,7 +1165,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
       <c r="B25" t="s">
         <v>6</v>
       </c>
@@ -1113,7 +1185,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
@@ -1130,7 +1205,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
@@ -1147,7 +1225,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
       <c r="B28" t="s">
         <v>6</v>
       </c>
@@ -1164,7 +1245,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
@@ -1181,7 +1265,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
@@ -1198,7 +1285,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -1215,7 +1305,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
@@ -1232,7 +1325,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -1249,7 +1345,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
       <c r="B34" t="s">
         <v>6</v>
       </c>
@@ -1266,7 +1365,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
       <c r="B35" t="s">
         <v>6</v>
       </c>
@@ -1283,7 +1385,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
       <c r="B36" t="s">
         <v>6</v>
       </c>
@@ -1300,7 +1405,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
       <c r="B37" t="s">
         <v>6</v>
       </c>
@@ -1317,7 +1425,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
@@ -1334,7 +1445,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
@@ -1351,7 +1465,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
       <c r="B40" t="s">
         <v>6</v>
       </c>
@@ -1368,7 +1485,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
       <c r="B41" t="s">
         <v>6</v>
       </c>
@@ -1385,7 +1505,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
       <c r="B42" t="s">
         <v>6</v>
       </c>
@@ -1402,7 +1525,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
       <c r="B43" t="s">
         <v>6</v>
       </c>
@@ -1419,7 +1545,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
       <c r="B44" t="s">
         <v>6</v>
       </c>
@@ -1436,7 +1565,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
       <c r="B45" t="s">
         <v>6</v>
       </c>
@@ -1453,7 +1585,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
       <c r="B46" t="s">
         <v>6</v>
       </c>
@@ -1470,7 +1605,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
       <c r="B47" t="s">
         <v>6</v>
       </c>
@@ -1487,7 +1625,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
       <c r="B48" t="s">
         <v>6</v>
       </c>
@@ -1505,6 +1646,9 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
       <c r="B49" t="s">
         <v>6</v>
       </c>
@@ -1522,6 +1666,9 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
       <c r="B50" t="s">
         <v>6</v>
       </c>
@@ -1539,6 +1686,9 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
       <c r="B51" t="s">
         <v>6</v>
       </c>
@@ -1556,6 +1706,9 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
       <c r="B52" t="s">
         <v>6</v>
       </c>
@@ -1573,6 +1726,9 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
       <c r="B53" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
chore: update dengue database 2022:2025
</commit_message>
<xml_diff>
--- a/data/bronze/dengue_prudente_weekly.xlsx
+++ b/data/bronze/dengue_prudente_weekly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryann\Documents\Projetos RStudio\dengue-project\data\bronze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28E787D-C558-4F74-8444-F2C8DF5F73C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE331FB-EBFD-4CDE-94E0-E42C9B391549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="188">
   <si>
     <t>Região|UF|Município</t>
   </si>
@@ -328,6 +328,270 @@
   </si>
   <si>
     <t>2024/52</t>
+  </si>
+  <si>
+    <t>2022/17</t>
+  </si>
+  <si>
+    <t>2022/18</t>
+  </si>
+  <si>
+    <t>2022/19</t>
+  </si>
+  <si>
+    <t>2022/20</t>
+  </si>
+  <si>
+    <t>2022/21</t>
+  </si>
+  <si>
+    <t>2022/22</t>
+  </si>
+  <si>
+    <t>2022/23</t>
+  </si>
+  <si>
+    <t>2022/24</t>
+  </si>
+  <si>
+    <t>2022/25</t>
+  </si>
+  <si>
+    <t>2022/26</t>
+  </si>
+  <si>
+    <t>2022/27</t>
+  </si>
+  <si>
+    <t>2022/28</t>
+  </si>
+  <si>
+    <t>2022/29</t>
+  </si>
+  <si>
+    <t>2022/30</t>
+  </si>
+  <si>
+    <t>2022/31</t>
+  </si>
+  <si>
+    <t>2022/32</t>
+  </si>
+  <si>
+    <t>2022/33</t>
+  </si>
+  <si>
+    <t>2022/34</t>
+  </si>
+  <si>
+    <t>2022/35</t>
+  </si>
+  <si>
+    <t>2022/36</t>
+  </si>
+  <si>
+    <t>2022/37</t>
+  </si>
+  <si>
+    <t>2022/38</t>
+  </si>
+  <si>
+    <t>2022/39</t>
+  </si>
+  <si>
+    <t>2022/40</t>
+  </si>
+  <si>
+    <t>2022/41</t>
+  </si>
+  <si>
+    <t>2022/42</t>
+  </si>
+  <si>
+    <t>2022/43</t>
+  </si>
+  <si>
+    <t>2022/44</t>
+  </si>
+  <si>
+    <t>2022/45</t>
+  </si>
+  <si>
+    <t>2022/46</t>
+  </si>
+  <si>
+    <t>2022/47</t>
+  </si>
+  <si>
+    <t>2022/48</t>
+  </si>
+  <si>
+    <t>2022/49</t>
+  </si>
+  <si>
+    <t>2022/50</t>
+  </si>
+  <si>
+    <t>2022/51</t>
+  </si>
+  <si>
+    <t>2022/52</t>
+  </si>
+  <si>
+    <t>2023/01</t>
+  </si>
+  <si>
+    <t>2023/02</t>
+  </si>
+  <si>
+    <t>2023/03</t>
+  </si>
+  <si>
+    <t>2023/04</t>
+  </si>
+  <si>
+    <t>2023/05</t>
+  </si>
+  <si>
+    <t>2023/06</t>
+  </si>
+  <si>
+    <t>2023/07</t>
+  </si>
+  <si>
+    <t>2023/08</t>
+  </si>
+  <si>
+    <t>2023/09</t>
+  </si>
+  <si>
+    <t>2023/10</t>
+  </si>
+  <si>
+    <t>2023/11</t>
+  </si>
+  <si>
+    <t>2023/12</t>
+  </si>
+  <si>
+    <t>2023/13</t>
+  </si>
+  <si>
+    <t>2023/14</t>
+  </si>
+  <si>
+    <t>2023/15</t>
+  </si>
+  <si>
+    <t>2023/16</t>
+  </si>
+  <si>
+    <t>2023/17</t>
+  </si>
+  <si>
+    <t>2023/18</t>
+  </si>
+  <si>
+    <t>2023/19</t>
+  </si>
+  <si>
+    <t>2023/20</t>
+  </si>
+  <si>
+    <t>2023/21</t>
+  </si>
+  <si>
+    <t>2023/22</t>
+  </si>
+  <si>
+    <t>2023/23</t>
+  </si>
+  <si>
+    <t>2023/24</t>
+  </si>
+  <si>
+    <t>2023/25</t>
+  </si>
+  <si>
+    <t>2023/26</t>
+  </si>
+  <si>
+    <t>2023/27</t>
+  </si>
+  <si>
+    <t>2023/28</t>
+  </si>
+  <si>
+    <t>2023/29</t>
+  </si>
+  <si>
+    <t>2023/30</t>
+  </si>
+  <si>
+    <t>2023/31</t>
+  </si>
+  <si>
+    <t>2023/32</t>
+  </si>
+  <si>
+    <t>2023/33</t>
+  </si>
+  <si>
+    <t>2023/34</t>
+  </si>
+  <si>
+    <t>2023/35</t>
+  </si>
+  <si>
+    <t>2023/36</t>
+  </si>
+  <si>
+    <t>2023/37</t>
+  </si>
+  <si>
+    <t>2023/38</t>
+  </si>
+  <si>
+    <t>2023/39</t>
+  </si>
+  <si>
+    <t>2023/40</t>
+  </si>
+  <si>
+    <t>2023/41</t>
+  </si>
+  <si>
+    <t>2023/42</t>
+  </si>
+  <si>
+    <t>2023/43</t>
+  </si>
+  <si>
+    <t>2023/44</t>
+  </si>
+  <si>
+    <t>2023/45</t>
+  </si>
+  <si>
+    <t>2023/46</t>
+  </si>
+  <si>
+    <t>2023/47</t>
+  </si>
+  <si>
+    <t>2023/48</t>
+  </si>
+  <si>
+    <t>2023/49</t>
+  </si>
+  <si>
+    <t>2023/50</t>
+  </si>
+  <si>
+    <t>2023/51</t>
+  </si>
+  <si>
+    <t>2023/52</t>
   </si>
 </sst>
 </file>
@@ -664,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,7 +943,7 @@
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
     <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.88671875" bestFit="1" customWidth="1"/>
@@ -713,16 +977,16 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>3541407</v>
+        <v>3541459</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="F2" s="1">
-        <v>7</v>
+        <v>766</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -733,16 +997,16 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>3541408</v>
+        <v>3541460</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="F3" s="1">
-        <v>3</v>
+        <v>926</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -753,16 +1017,16 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>3541409</v>
+        <v>3541461</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="F4" s="1">
-        <v>4</v>
+        <v>674</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -773,16 +1037,16 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>3541410</v>
+        <v>3541462</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="F5" s="1">
-        <v>7</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -793,16 +1057,16 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>3541411</v>
+        <v>3541463</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="F6" s="1">
-        <v>5</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -813,16 +1077,16 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>3541412</v>
+        <v>3541464</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F7" s="1">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -833,16 +1097,16 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>3541413</v>
+        <v>3541465</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1">
-        <v>11</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -853,16 +1117,16 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>3541414</v>
+        <v>3541466</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="F9" s="1">
-        <v>9</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -873,16 +1137,16 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>3541415</v>
+        <v>3541467</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="F10" s="1">
-        <v>10</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -893,16 +1157,16 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>3541416</v>
+        <v>3541468</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="F11" s="1">
-        <v>10</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -913,16 +1177,16 @@
         <v>6</v>
       </c>
       <c r="C12">
-        <v>3541417</v>
+        <v>3541469</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="F12" s="1">
-        <v>10</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -933,16 +1197,16 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>3541418</v>
+        <v>3541470</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="F13" s="1">
-        <v>15</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -953,16 +1217,16 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>3541419</v>
+        <v>3541471</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="F14" s="1">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -973,16 +1237,16 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <v>3541420</v>
+        <v>3541472</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="F15" s="1">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -993,16 +1257,16 @@
         <v>6</v>
       </c>
       <c r="C16">
-        <v>3541421</v>
+        <v>3541473</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="F16" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1013,16 +1277,16 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>3541422</v>
+        <v>3541474</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="F17" s="1">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1033,16 +1297,16 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>3541423</v>
+        <v>3541475</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="F18" s="1">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1053,16 +1317,16 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>3541424</v>
+        <v>3541476</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="F19" s="1">
-        <v>73</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1073,16 +1337,16 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>3541425</v>
+        <v>3541477</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="F20" s="1">
-        <v>89</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1093,16 +1357,16 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>3541426</v>
+        <v>3541478</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="F21" s="1">
-        <v>106</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1113,16 +1377,16 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <v>3541427</v>
+        <v>3541479</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="F22" s="1">
-        <v>76</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1133,16 +1397,16 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <v>3541428</v>
+        <v>3541480</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="F23" s="1">
-        <v>58</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1153,16 +1417,16 @@
         <v>6</v>
       </c>
       <c r="C24">
-        <v>3541429</v>
+        <v>3541481</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="F24" s="1">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1173,16 +1437,16 @@
         <v>6</v>
       </c>
       <c r="C25">
-        <v>3541430</v>
+        <v>3541482</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="F25" s="1">
-        <v>56</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1193,16 +1457,16 @@
         <v>6</v>
       </c>
       <c r="C26">
-        <v>3541431</v>
+        <v>3541483</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="F26" s="1">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1213,16 +1477,16 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <v>3541432</v>
+        <v>3541484</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="F27" s="1">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1233,16 +1497,16 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>3541433</v>
+        <v>3541485</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="F28" s="1">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1253,16 +1517,16 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>3541434</v>
+        <v>3541486</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="F29" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1273,16 +1537,16 @@
         <v>6</v>
       </c>
       <c r="C30">
-        <v>3541435</v>
+        <v>3541487</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="F30" s="1">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1293,16 +1557,16 @@
         <v>6</v>
       </c>
       <c r="C31">
-        <v>3541436</v>
+        <v>3541488</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="F31" s="1">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1313,16 +1577,16 @@
         <v>6</v>
       </c>
       <c r="C32">
-        <v>3541437</v>
+        <v>3541489</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="F32" s="1">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1333,16 +1597,16 @@
         <v>6</v>
       </c>
       <c r="C33">
-        <v>3541438</v>
+        <v>3541490</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="F33" s="1">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1353,16 +1617,16 @@
         <v>6</v>
       </c>
       <c r="C34">
-        <v>3541439</v>
+        <v>3541491</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="F34" s="1">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1373,16 +1637,16 @@
         <v>6</v>
       </c>
       <c r="C35">
-        <v>3541440</v>
+        <v>3541492</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="F35" s="1">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1393,16 +1657,16 @@
         <v>6</v>
       </c>
       <c r="C36">
-        <v>3541441</v>
+        <v>3541493</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="F36" s="1">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1413,16 +1677,16 @@
         <v>6</v>
       </c>
       <c r="C37">
-        <v>3541442</v>
+        <v>3541494</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="F37" s="1">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1433,16 +1697,16 @@
         <v>6</v>
       </c>
       <c r="C38">
-        <v>3541443</v>
+        <v>3541407</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="F38" s="1">
-        <v>9</v>
+        <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1453,16 +1717,16 @@
         <v>6</v>
       </c>
       <c r="C39">
-        <v>3541444</v>
+        <v>3541408</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="F39" s="1">
-        <v>6</v>
+        <v>357</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1473,16 +1737,16 @@
         <v>6</v>
       </c>
       <c r="C40">
-        <v>3541445</v>
+        <v>3541409</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="F40" s="1">
-        <v>13</v>
+        <v>410</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1493,16 +1757,16 @@
         <v>6</v>
       </c>
       <c r="C41">
-        <v>3541446</v>
+        <v>3541410</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="F41" s="1">
-        <v>2</v>
+        <v>601</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,16 +1777,16 @@
         <v>6</v>
       </c>
       <c r="C42">
-        <v>3541447</v>
+        <v>3541411</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="F42" s="1">
-        <v>6</v>
+        <v>782</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1533,16 +1797,16 @@
         <v>6</v>
       </c>
       <c r="C43">
-        <v>3541448</v>
+        <v>3541412</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="F43" s="1">
-        <v>9</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1553,16 +1817,16 @@
         <v>6</v>
       </c>
       <c r="C44">
-        <v>3541449</v>
+        <v>3541413</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="F44" s="1">
-        <v>4</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1573,16 +1837,16 @@
         <v>6</v>
       </c>
       <c r="C45">
-        <v>3541450</v>
+        <v>3541414</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="F45" s="1">
-        <v>5</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1593,16 +1857,16 @@
         <v>6</v>
       </c>
       <c r="C46">
-        <v>3541451</v>
+        <v>3541415</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
       </c>
       <c r="E46" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="F46" s="1">
-        <v>5</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1613,16 +1877,16 @@
         <v>6</v>
       </c>
       <c r="C47">
-        <v>3541452</v>
+        <v>3541416</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="F47" s="1">
-        <v>9</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1633,16 +1897,16 @@
         <v>6</v>
       </c>
       <c r="C48">
-        <v>3541453</v>
+        <v>3541417</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="F48" s="1">
-        <v>17</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1653,16 +1917,16 @@
         <v>6</v>
       </c>
       <c r="C49">
-        <v>3541454</v>
+        <v>3541418</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="F49" s="1">
-        <v>13</v>
+        <v>3321</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1673,16 +1937,16 @@
         <v>6</v>
       </c>
       <c r="C50">
-        <v>3541455</v>
+        <v>3541419</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
       </c>
       <c r="E50" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="F50" s="1">
-        <v>21</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1693,16 +1957,16 @@
         <v>6</v>
       </c>
       <c r="C51">
-        <v>3541456</v>
+        <v>3541420</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="F51" s="1">
-        <v>40</v>
+        <v>3144</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1713,16 +1977,16 @@
         <v>6</v>
       </c>
       <c r="C52">
-        <v>3541457</v>
+        <v>3541421</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
       </c>
       <c r="E52" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="F52" s="1">
-        <v>39</v>
+        <v>2966</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1733,16 +1997,16 @@
         <v>6</v>
       </c>
       <c r="C53">
-        <v>3541458</v>
+        <v>3541422</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="F53" s="1">
-        <v>33</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1753,16 +2017,16 @@
         <v>6</v>
       </c>
       <c r="C54">
-        <v>3541406</v>
+        <v>3541423</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="F54" s="1">
-        <v>126</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1773,16 +2037,16 @@
         <v>6</v>
       </c>
       <c r="C55">
-        <v>3541406</v>
+        <v>3541424</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
       </c>
       <c r="E55" t="s">
-        <v>9</v>
+        <v>153</v>
       </c>
       <c r="F55" s="1">
-        <v>158</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1793,16 +2057,16 @@
         <v>6</v>
       </c>
       <c r="C56">
-        <v>3541406</v>
+        <v>3541425</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>10</v>
+        <v>154</v>
       </c>
       <c r="F56" s="1">
-        <v>301</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1813,16 +2077,16 @@
         <v>6</v>
       </c>
       <c r="C57">
-        <v>3541406</v>
+        <v>3541426</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>155</v>
       </c>
       <c r="F57" s="1">
-        <v>381</v>
+        <v>847</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1833,16 +2097,16 @@
         <v>6</v>
       </c>
       <c r="C58">
-        <v>3541406</v>
+        <v>3541427</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="F58" s="1">
-        <v>763</v>
+        <v>471</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1853,16 +2117,16 @@
         <v>6</v>
       </c>
       <c r="C59">
-        <v>3541406</v>
+        <v>3541428</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="F59" s="1">
-        <v>1284</v>
+        <v>325</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1873,16 +2137,16 @@
         <v>6</v>
       </c>
       <c r="C60">
-        <v>3541406</v>
+        <v>3541429</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="F60" s="1">
-        <v>2079</v>
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1893,16 +2157,16 @@
         <v>6</v>
       </c>
       <c r="C61">
-        <v>3541406</v>
+        <v>3541430</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>15</v>
+        <v>159</v>
       </c>
       <c r="F61" s="1">
-        <v>2650</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1913,16 +2177,16 @@
         <v>6</v>
       </c>
       <c r="C62">
-        <v>3541406</v>
+        <v>3541431</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>16</v>
+        <v>160</v>
       </c>
       <c r="F62" s="1">
-        <v>2949</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1933,16 +2197,16 @@
         <v>6</v>
       </c>
       <c r="C63">
-        <v>3541406</v>
+        <v>3541432</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>17</v>
+        <v>161</v>
       </c>
       <c r="F63" s="1">
-        <v>2697</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1953,16 +2217,16 @@
         <v>6</v>
       </c>
       <c r="C64">
-        <v>3541406</v>
+        <v>3541433</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>18</v>
+        <v>162</v>
       </c>
       <c r="F64" s="1">
-        <v>2588</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1973,16 +2237,16 @@
         <v>6</v>
       </c>
       <c r="C65">
-        <v>3541406</v>
+        <v>3541434</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>19</v>
+        <v>163</v>
       </c>
       <c r="F65" s="1">
-        <v>2534</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1993,16 +2257,16 @@
         <v>6</v>
       </c>
       <c r="C66">
-        <v>3541406</v>
+        <v>3541435</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>20</v>
+        <v>164</v>
       </c>
       <c r="F66" s="1">
-        <v>2052</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2013,16 +2277,16 @@
         <v>6</v>
       </c>
       <c r="C67">
-        <v>3541406</v>
+        <v>3541436</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
       </c>
       <c r="E67" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="F67" s="1">
-        <v>1502</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2033,16 +2297,16 @@
         <v>6</v>
       </c>
       <c r="C68">
-        <v>3541406</v>
+        <v>3541437</v>
       </c>
       <c r="D68" t="s">
         <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>22</v>
+        <v>166</v>
       </c>
       <c r="F68" s="1">
-        <v>1168</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2053,16 +2317,16 @@
         <v>6</v>
       </c>
       <c r="C69">
-        <v>3541406</v>
+        <v>3541438</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
       </c>
       <c r="E69" t="s">
-        <v>23</v>
+        <v>167</v>
       </c>
       <c r="F69" s="1">
-        <v>821</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2073,16 +2337,16 @@
         <v>6</v>
       </c>
       <c r="C70">
-        <v>3541406</v>
+        <v>3541439</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F70" s="1">
-        <v>674</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2093,16 +2357,16 @@
         <v>6</v>
       </c>
       <c r="C71">
-        <v>3541406</v>
+        <v>3541440</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
       </c>
       <c r="E71" t="s">
-        <v>25</v>
+        <v>169</v>
       </c>
       <c r="F71" s="1">
-        <v>533</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2113,16 +2377,16 @@
         <v>6</v>
       </c>
       <c r="C72">
-        <v>3541406</v>
+        <v>3541441</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
       </c>
       <c r="E72" t="s">
-        <v>26</v>
+        <v>170</v>
       </c>
       <c r="F72" s="1">
-        <v>492</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2133,16 +2397,16 @@
         <v>6</v>
       </c>
       <c r="C73">
-        <v>3541406</v>
+        <v>3541442</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
       </c>
       <c r="E73" t="s">
-        <v>27</v>
+        <v>171</v>
       </c>
       <c r="F73" s="1">
-        <v>383</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2153,16 +2417,16 @@
         <v>6</v>
       </c>
       <c r="C74">
-        <v>3541406</v>
+        <v>3541443</v>
       </c>
       <c r="D74" t="s">
         <v>7</v>
       </c>
       <c r="E74" t="s">
-        <v>28</v>
+        <v>172</v>
       </c>
       <c r="F74" s="1">
-        <v>357</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2173,16 +2437,16 @@
         <v>6</v>
       </c>
       <c r="C75">
-        <v>3541406</v>
+        <v>3541444</v>
       </c>
       <c r="D75" t="s">
         <v>7</v>
       </c>
       <c r="E75" t="s">
-        <v>29</v>
+        <v>173</v>
       </c>
       <c r="F75" s="1">
-        <v>275</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2193,16 +2457,16 @@
         <v>6</v>
       </c>
       <c r="C76">
-        <v>3541406</v>
+        <v>3541445</v>
       </c>
       <c r="D76" t="s">
         <v>7</v>
       </c>
       <c r="E76" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
       <c r="F76" s="1">
-        <v>264</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2213,16 +2477,16 @@
         <v>6</v>
       </c>
       <c r="C77">
-        <v>3541406</v>
+        <v>3541446</v>
       </c>
       <c r="D77" t="s">
         <v>7</v>
       </c>
       <c r="E77" t="s">
-        <v>31</v>
+        <v>175</v>
       </c>
       <c r="F77" s="1">
-        <v>155</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2233,16 +2497,16 @@
         <v>6</v>
       </c>
       <c r="C78">
-        <v>3541406</v>
+        <v>3541447</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
       </c>
       <c r="E78" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
       <c r="F78" s="1">
-        <v>117</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2253,16 +2517,16 @@
         <v>6</v>
       </c>
       <c r="C79">
-        <v>3541406</v>
+        <v>3541448</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
       </c>
       <c r="E79" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="F79" s="1">
-        <v>119</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2273,16 +2537,16 @@
         <v>6</v>
       </c>
       <c r="C80">
-        <v>3541406</v>
+        <v>3541449</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
       </c>
       <c r="E80" t="s">
-        <v>34</v>
+        <v>178</v>
       </c>
       <c r="F80" s="1">
-        <v>74</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2293,16 +2557,16 @@
         <v>6</v>
       </c>
       <c r="C81">
-        <v>3541406</v>
+        <v>3541450</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
       </c>
       <c r="E81" t="s">
-        <v>35</v>
+        <v>179</v>
       </c>
       <c r="F81" s="1">
-        <v>96</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2313,16 +2577,16 @@
         <v>6</v>
       </c>
       <c r="C82">
-        <v>3541406</v>
+        <v>3541451</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
       </c>
       <c r="E82" t="s">
-        <v>36</v>
+        <v>180</v>
       </c>
       <c r="F82" s="1">
-        <v>98</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2333,16 +2597,16 @@
         <v>6</v>
       </c>
       <c r="C83">
-        <v>3541406</v>
+        <v>3541452</v>
       </c>
       <c r="D83" t="s">
         <v>7</v>
       </c>
       <c r="E83" t="s">
-        <v>37</v>
+        <v>181</v>
       </c>
       <c r="F83" s="1">
-        <v>61</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2353,16 +2617,16 @@
         <v>6</v>
       </c>
       <c r="C84">
-        <v>3541406</v>
+        <v>3541453</v>
       </c>
       <c r="D84" t="s">
         <v>7</v>
       </c>
       <c r="E84" t="s">
-        <v>38</v>
+        <v>182</v>
       </c>
       <c r="F84" s="1">
-        <v>59</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2373,16 +2637,16 @@
         <v>6</v>
       </c>
       <c r="C85">
-        <v>3541406</v>
+        <v>3541454</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
       </c>
       <c r="E85" t="s">
-        <v>39</v>
+        <v>183</v>
       </c>
       <c r="F85" s="1">
-        <v>44</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2393,16 +2657,16 @@
         <v>6</v>
       </c>
       <c r="C86">
-        <v>3541406</v>
+        <v>3541455</v>
       </c>
       <c r="D86" t="s">
         <v>7</v>
       </c>
       <c r="E86" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="F86" s="1">
-        <v>71</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2413,16 +2677,16 @@
         <v>6</v>
       </c>
       <c r="C87">
-        <v>3541406</v>
+        <v>3541456</v>
       </c>
       <c r="D87" t="s">
         <v>7</v>
       </c>
       <c r="E87" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
       <c r="F87" s="1">
-        <v>95</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2433,16 +2697,16 @@
         <v>6</v>
       </c>
       <c r="C88">
-        <v>3541406</v>
+        <v>3541457</v>
       </c>
       <c r="D88" t="s">
         <v>7</v>
       </c>
       <c r="E88" t="s">
-        <v>42</v>
+        <v>186</v>
       </c>
       <c r="F88" s="1">
-        <v>96</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2453,16 +2717,16 @@
         <v>6</v>
       </c>
       <c r="C89">
-        <v>3541406</v>
+        <v>3541458</v>
       </c>
       <c r="D89" t="s">
         <v>7</v>
       </c>
       <c r="E89" t="s">
-        <v>43</v>
+        <v>187</v>
       </c>
       <c r="F89" s="1">
-        <v>85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2473,16 +2737,16 @@
         <v>6</v>
       </c>
       <c r="C90">
-        <v>3541406</v>
+        <v>3541407</v>
       </c>
       <c r="D90" t="s">
         <v>7</v>
       </c>
       <c r="E90" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F90" s="1">
-        <v>94</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2493,16 +2757,16 @@
         <v>6</v>
       </c>
       <c r="C91">
-        <v>3541406</v>
+        <v>3541408</v>
       </c>
       <c r="D91" t="s">
         <v>7</v>
       </c>
       <c r="E91" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F91" s="1">
-        <v>72</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2513,21 +2777,1781 @@
         <v>6</v>
       </c>
       <c r="C92">
+        <v>3541409</v>
+      </c>
+      <c r="D92" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" t="s">
+        <v>50</v>
+      </c>
+      <c r="F92" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93">
+        <v>3541410</v>
+      </c>
+      <c r="D93" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" t="s">
+        <v>51</v>
+      </c>
+      <c r="F93" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94">
+        <v>3541411</v>
+      </c>
+      <c r="D94" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" t="s">
+        <v>52</v>
+      </c>
+      <c r="F94" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95">
+        <v>3541412</v>
+      </c>
+      <c r="D95" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" t="s">
+        <v>53</v>
+      </c>
+      <c r="F95" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96">
+        <v>3541413</v>
+      </c>
+      <c r="D96" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" t="s">
+        <v>54</v>
+      </c>
+      <c r="F96" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97">
+        <v>3541414</v>
+      </c>
+      <c r="D97" t="s">
+        <v>7</v>
+      </c>
+      <c r="E97" t="s">
+        <v>55</v>
+      </c>
+      <c r="F97" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98">
+        <v>3541415</v>
+      </c>
+      <c r="D98" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" t="s">
+        <v>56</v>
+      </c>
+      <c r="F98" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99">
+        <v>3541416</v>
+      </c>
+      <c r="D99" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" t="s">
+        <v>57</v>
+      </c>
+      <c r="F99" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100">
+        <v>3541417</v>
+      </c>
+      <c r="D100" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" t="s">
+        <v>58</v>
+      </c>
+      <c r="F100" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101">
+        <v>3541418</v>
+      </c>
+      <c r="D101" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" t="s">
+        <v>59</v>
+      </c>
+      <c r="F101" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" t="s">
+        <v>6</v>
+      </c>
+      <c r="C102">
+        <v>3541419</v>
+      </c>
+      <c r="D102" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" t="s">
+        <v>60</v>
+      </c>
+      <c r="F102" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103">
+        <v>3541420</v>
+      </c>
+      <c r="D103" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" t="s">
+        <v>61</v>
+      </c>
+      <c r="F103" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104">
+        <v>3541421</v>
+      </c>
+      <c r="D104" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" t="s">
+        <v>62</v>
+      </c>
+      <c r="F104" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" t="s">
+        <v>6</v>
+      </c>
+      <c r="C105">
+        <v>3541422</v>
+      </c>
+      <c r="D105" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" t="s">
+        <v>63</v>
+      </c>
+      <c r="F105" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" t="s">
+        <v>6</v>
+      </c>
+      <c r="C106">
+        <v>3541423</v>
+      </c>
+      <c r="D106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" t="s">
+        <v>64</v>
+      </c>
+      <c r="F106" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107">
+        <v>3541424</v>
+      </c>
+      <c r="D107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" t="s">
+        <v>65</v>
+      </c>
+      <c r="F107" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108">
+        <v>3541425</v>
+      </c>
+      <c r="D108" t="s">
+        <v>7</v>
+      </c>
+      <c r="E108" t="s">
+        <v>66</v>
+      </c>
+      <c r="F108" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109">
+        <v>3541426</v>
+      </c>
+      <c r="D109" t="s">
+        <v>7</v>
+      </c>
+      <c r="E109" t="s">
+        <v>67</v>
+      </c>
+      <c r="F109" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110">
+        <v>3541427</v>
+      </c>
+      <c r="D110" t="s">
+        <v>7</v>
+      </c>
+      <c r="E110" t="s">
+        <v>68</v>
+      </c>
+      <c r="F110" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>5</v>
+      </c>
+      <c r="B111" t="s">
+        <v>6</v>
+      </c>
+      <c r="C111">
+        <v>3541428</v>
+      </c>
+      <c r="D111" t="s">
+        <v>7</v>
+      </c>
+      <c r="E111" t="s">
+        <v>69</v>
+      </c>
+      <c r="F111" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" t="s">
+        <v>6</v>
+      </c>
+      <c r="C112">
+        <v>3541429</v>
+      </c>
+      <c r="D112" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" t="s">
+        <v>70</v>
+      </c>
+      <c r="F112" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113" t="s">
+        <v>6</v>
+      </c>
+      <c r="C113">
+        <v>3541430</v>
+      </c>
+      <c r="D113" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" t="s">
+        <v>71</v>
+      </c>
+      <c r="F113" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>5</v>
+      </c>
+      <c r="B114" t="s">
+        <v>6</v>
+      </c>
+      <c r="C114">
+        <v>3541431</v>
+      </c>
+      <c r="D114" t="s">
+        <v>7</v>
+      </c>
+      <c r="E114" t="s">
+        <v>72</v>
+      </c>
+      <c r="F114" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115" t="s">
+        <v>6</v>
+      </c>
+      <c r="C115">
+        <v>3541432</v>
+      </c>
+      <c r="D115" t="s">
+        <v>7</v>
+      </c>
+      <c r="E115" t="s">
+        <v>73</v>
+      </c>
+      <c r="F115" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116">
+        <v>3541433</v>
+      </c>
+      <c r="D116" t="s">
+        <v>7</v>
+      </c>
+      <c r="E116" t="s">
+        <v>74</v>
+      </c>
+      <c r="F116" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117">
+        <v>3541434</v>
+      </c>
+      <c r="D117" t="s">
+        <v>7</v>
+      </c>
+      <c r="E117" t="s">
+        <v>75</v>
+      </c>
+      <c r="F117" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118">
+        <v>3541435</v>
+      </c>
+      <c r="D118" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" t="s">
+        <v>76</v>
+      </c>
+      <c r="F118" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>5</v>
+      </c>
+      <c r="B119" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119">
+        <v>3541436</v>
+      </c>
+      <c r="D119" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" t="s">
+        <v>77</v>
+      </c>
+      <c r="F119" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" t="s">
+        <v>6</v>
+      </c>
+      <c r="C120">
+        <v>3541437</v>
+      </c>
+      <c r="D120" t="s">
+        <v>7</v>
+      </c>
+      <c r="E120" t="s">
+        <v>78</v>
+      </c>
+      <c r="F120" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121">
+        <v>3541438</v>
+      </c>
+      <c r="D121" t="s">
+        <v>7</v>
+      </c>
+      <c r="E121" t="s">
+        <v>79</v>
+      </c>
+      <c r="F121" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>5</v>
+      </c>
+      <c r="B122" t="s">
+        <v>6</v>
+      </c>
+      <c r="C122">
+        <v>3541439</v>
+      </c>
+      <c r="D122" t="s">
+        <v>7</v>
+      </c>
+      <c r="E122" t="s">
+        <v>80</v>
+      </c>
+      <c r="F122" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>5</v>
+      </c>
+      <c r="B123" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123">
+        <v>3541440</v>
+      </c>
+      <c r="D123" t="s">
+        <v>7</v>
+      </c>
+      <c r="E123" t="s">
+        <v>81</v>
+      </c>
+      <c r="F123" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124">
+        <v>3541441</v>
+      </c>
+      <c r="D124" t="s">
+        <v>7</v>
+      </c>
+      <c r="E124" t="s">
+        <v>82</v>
+      </c>
+      <c r="F124" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>5</v>
+      </c>
+      <c r="B125" t="s">
+        <v>6</v>
+      </c>
+      <c r="C125">
+        <v>3541442</v>
+      </c>
+      <c r="D125" t="s">
+        <v>7</v>
+      </c>
+      <c r="E125" t="s">
+        <v>83</v>
+      </c>
+      <c r="F125" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>5</v>
+      </c>
+      <c r="B126" t="s">
+        <v>6</v>
+      </c>
+      <c r="C126">
+        <v>3541443</v>
+      </c>
+      <c r="D126" t="s">
+        <v>7</v>
+      </c>
+      <c r="E126" t="s">
+        <v>84</v>
+      </c>
+      <c r="F126" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>5</v>
+      </c>
+      <c r="B127" t="s">
+        <v>6</v>
+      </c>
+      <c r="C127">
+        <v>3541444</v>
+      </c>
+      <c r="D127" t="s">
+        <v>7</v>
+      </c>
+      <c r="E127" t="s">
+        <v>85</v>
+      </c>
+      <c r="F127" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>5</v>
+      </c>
+      <c r="B128" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128">
+        <v>3541445</v>
+      </c>
+      <c r="D128" t="s">
+        <v>7</v>
+      </c>
+      <c r="E128" t="s">
+        <v>86</v>
+      </c>
+      <c r="F128" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>5</v>
+      </c>
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129">
+        <v>3541446</v>
+      </c>
+      <c r="D129" t="s">
+        <v>7</v>
+      </c>
+      <c r="E129" t="s">
+        <v>87</v>
+      </c>
+      <c r="F129" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>5</v>
+      </c>
+      <c r="B130" t="s">
+        <v>6</v>
+      </c>
+      <c r="C130">
+        <v>3541447</v>
+      </c>
+      <c r="D130" t="s">
+        <v>7</v>
+      </c>
+      <c r="E130" t="s">
+        <v>88</v>
+      </c>
+      <c r="F130" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>5</v>
+      </c>
+      <c r="B131" t="s">
+        <v>6</v>
+      </c>
+      <c r="C131">
+        <v>3541448</v>
+      </c>
+      <c r="D131" t="s">
+        <v>7</v>
+      </c>
+      <c r="E131" t="s">
+        <v>89</v>
+      </c>
+      <c r="F131" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>5</v>
+      </c>
+      <c r="B132" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132">
+        <v>3541449</v>
+      </c>
+      <c r="D132" t="s">
+        <v>7</v>
+      </c>
+      <c r="E132" t="s">
+        <v>90</v>
+      </c>
+      <c r="F132" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>5</v>
+      </c>
+      <c r="B133" t="s">
+        <v>6</v>
+      </c>
+      <c r="C133">
+        <v>3541450</v>
+      </c>
+      <c r="D133" t="s">
+        <v>7</v>
+      </c>
+      <c r="E133" t="s">
+        <v>91</v>
+      </c>
+      <c r="F133" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>5</v>
+      </c>
+      <c r="B134" t="s">
+        <v>6</v>
+      </c>
+      <c r="C134">
+        <v>3541451</v>
+      </c>
+      <c r="D134" t="s">
+        <v>7</v>
+      </c>
+      <c r="E134" t="s">
+        <v>92</v>
+      </c>
+      <c r="F134" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>5</v>
+      </c>
+      <c r="B135" t="s">
+        <v>6</v>
+      </c>
+      <c r="C135">
+        <v>3541452</v>
+      </c>
+      <c r="D135" t="s">
+        <v>7</v>
+      </c>
+      <c r="E135" t="s">
+        <v>93</v>
+      </c>
+      <c r="F135" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>5</v>
+      </c>
+      <c r="B136" t="s">
+        <v>6</v>
+      </c>
+      <c r="C136">
+        <v>3541453</v>
+      </c>
+      <c r="D136" t="s">
+        <v>7</v>
+      </c>
+      <c r="E136" t="s">
+        <v>94</v>
+      </c>
+      <c r="F136" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>5</v>
+      </c>
+      <c r="B137" t="s">
+        <v>6</v>
+      </c>
+      <c r="C137">
+        <v>3541454</v>
+      </c>
+      <c r="D137" t="s">
+        <v>7</v>
+      </c>
+      <c r="E137" t="s">
+        <v>95</v>
+      </c>
+      <c r="F137" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>5</v>
+      </c>
+      <c r="B138" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138">
+        <v>3541455</v>
+      </c>
+      <c r="D138" t="s">
+        <v>7</v>
+      </c>
+      <c r="E138" t="s">
+        <v>96</v>
+      </c>
+      <c r="F138" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>5</v>
+      </c>
+      <c r="B139" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139">
+        <v>3541456</v>
+      </c>
+      <c r="D139" t="s">
+        <v>7</v>
+      </c>
+      <c r="E139" t="s">
+        <v>97</v>
+      </c>
+      <c r="F139" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>5</v>
+      </c>
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140">
+        <v>3541457</v>
+      </c>
+      <c r="D140" t="s">
+        <v>7</v>
+      </c>
+      <c r="E140" t="s">
+        <v>98</v>
+      </c>
+      <c r="F140" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>5</v>
+      </c>
+      <c r="B141" t="s">
+        <v>6</v>
+      </c>
+      <c r="C141">
+        <v>3541458</v>
+      </c>
+      <c r="D141" t="s">
+        <v>7</v>
+      </c>
+      <c r="E141" t="s">
+        <v>99</v>
+      </c>
+      <c r="F141" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>5</v>
+      </c>
+      <c r="B142" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142">
         <v>3541406</v>
       </c>
-      <c r="D92" t="s">
-        <v>7</v>
-      </c>
-      <c r="E92" t="s">
+      <c r="D142" t="s">
+        <v>7</v>
+      </c>
+      <c r="E142" t="s">
+        <v>8</v>
+      </c>
+      <c r="F142" s="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>5</v>
+      </c>
+      <c r="B143" t="s">
+        <v>6</v>
+      </c>
+      <c r="C143">
+        <v>3541406</v>
+      </c>
+      <c r="D143" t="s">
+        <v>7</v>
+      </c>
+      <c r="E143" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" s="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>5</v>
+      </c>
+      <c r="B144" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144">
+        <v>3541406</v>
+      </c>
+      <c r="D144" t="s">
+        <v>7</v>
+      </c>
+      <c r="E144" t="s">
+        <v>10</v>
+      </c>
+      <c r="F144" s="1">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>5</v>
+      </c>
+      <c r="B145" t="s">
+        <v>6</v>
+      </c>
+      <c r="C145">
+        <v>3541406</v>
+      </c>
+      <c r="D145" t="s">
+        <v>7</v>
+      </c>
+      <c r="E145" t="s">
+        <v>11</v>
+      </c>
+      <c r="F145" s="1">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>5</v>
+      </c>
+      <c r="B146" t="s">
+        <v>6</v>
+      </c>
+      <c r="C146">
+        <v>3541406</v>
+      </c>
+      <c r="D146" t="s">
+        <v>7</v>
+      </c>
+      <c r="E146" t="s">
+        <v>12</v>
+      </c>
+      <c r="F146" s="1">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>5</v>
+      </c>
+      <c r="B147" t="s">
+        <v>6</v>
+      </c>
+      <c r="C147">
+        <v>3541406</v>
+      </c>
+      <c r="D147" t="s">
+        <v>7</v>
+      </c>
+      <c r="E147" t="s">
+        <v>13</v>
+      </c>
+      <c r="F147" s="1">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>5</v>
+      </c>
+      <c r="B148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148">
+        <v>3541406</v>
+      </c>
+      <c r="D148" t="s">
+        <v>7</v>
+      </c>
+      <c r="E148" t="s">
+        <v>14</v>
+      </c>
+      <c r="F148" s="1">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>5</v>
+      </c>
+      <c r="B149" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149">
+        <v>3541406</v>
+      </c>
+      <c r="D149" t="s">
+        <v>7</v>
+      </c>
+      <c r="E149" t="s">
+        <v>15</v>
+      </c>
+      <c r="F149" s="1">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>5</v>
+      </c>
+      <c r="B150" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150">
+        <v>3541406</v>
+      </c>
+      <c r="D150" t="s">
+        <v>7</v>
+      </c>
+      <c r="E150" t="s">
+        <v>16</v>
+      </c>
+      <c r="F150" s="1">
+        <v>2949</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>5</v>
+      </c>
+      <c r="B151" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151">
+        <v>3541406</v>
+      </c>
+      <c r="D151" t="s">
+        <v>7</v>
+      </c>
+      <c r="E151" t="s">
+        <v>17</v>
+      </c>
+      <c r="F151" s="1">
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>5</v>
+      </c>
+      <c r="B152" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152">
+        <v>3541406</v>
+      </c>
+      <c r="D152" t="s">
+        <v>7</v>
+      </c>
+      <c r="E152" t="s">
+        <v>18</v>
+      </c>
+      <c r="F152" s="1">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>5</v>
+      </c>
+      <c r="B153" t="s">
+        <v>6</v>
+      </c>
+      <c r="C153">
+        <v>3541406</v>
+      </c>
+      <c r="D153" t="s">
+        <v>7</v>
+      </c>
+      <c r="E153" t="s">
+        <v>19</v>
+      </c>
+      <c r="F153" s="1">
+        <v>2534</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>5</v>
+      </c>
+      <c r="B154" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154">
+        <v>3541406</v>
+      </c>
+      <c r="D154" t="s">
+        <v>7</v>
+      </c>
+      <c r="E154" t="s">
+        <v>20</v>
+      </c>
+      <c r="F154" s="1">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>5</v>
+      </c>
+      <c r="B155" t="s">
+        <v>6</v>
+      </c>
+      <c r="C155">
+        <v>3541406</v>
+      </c>
+      <c r="D155" t="s">
+        <v>7</v>
+      </c>
+      <c r="E155" t="s">
+        <v>21</v>
+      </c>
+      <c r="F155" s="1">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>5</v>
+      </c>
+      <c r="B156" t="s">
+        <v>6</v>
+      </c>
+      <c r="C156">
+        <v>3541406</v>
+      </c>
+      <c r="D156" t="s">
+        <v>7</v>
+      </c>
+      <c r="E156" t="s">
+        <v>22</v>
+      </c>
+      <c r="F156" s="1">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>5</v>
+      </c>
+      <c r="B157" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157">
+        <v>3541406</v>
+      </c>
+      <c r="D157" t="s">
+        <v>7</v>
+      </c>
+      <c r="E157" t="s">
+        <v>23</v>
+      </c>
+      <c r="F157" s="1">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>5</v>
+      </c>
+      <c r="B158" t="s">
+        <v>6</v>
+      </c>
+      <c r="C158">
+        <v>3541406</v>
+      </c>
+      <c r="D158" t="s">
+        <v>7</v>
+      </c>
+      <c r="E158" t="s">
+        <v>24</v>
+      </c>
+      <c r="F158" s="1">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>5</v>
+      </c>
+      <c r="B159" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159">
+        <v>3541406</v>
+      </c>
+      <c r="D159" t="s">
+        <v>7</v>
+      </c>
+      <c r="E159" t="s">
+        <v>25</v>
+      </c>
+      <c r="F159" s="1">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>5</v>
+      </c>
+      <c r="B160" t="s">
+        <v>6</v>
+      </c>
+      <c r="C160">
+        <v>3541406</v>
+      </c>
+      <c r="D160" t="s">
+        <v>7</v>
+      </c>
+      <c r="E160" t="s">
+        <v>26</v>
+      </c>
+      <c r="F160" s="1">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161" t="s">
+        <v>6</v>
+      </c>
+      <c r="C161">
+        <v>3541406</v>
+      </c>
+      <c r="D161" t="s">
+        <v>7</v>
+      </c>
+      <c r="E161" t="s">
+        <v>27</v>
+      </c>
+      <c r="F161" s="1">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162" t="s">
+        <v>6</v>
+      </c>
+      <c r="C162">
+        <v>3541406</v>
+      </c>
+      <c r="D162" t="s">
+        <v>7</v>
+      </c>
+      <c r="E162" t="s">
+        <v>28</v>
+      </c>
+      <c r="F162" s="1">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>5</v>
+      </c>
+      <c r="B163" t="s">
+        <v>6</v>
+      </c>
+      <c r="C163">
+        <v>3541406</v>
+      </c>
+      <c r="D163" t="s">
+        <v>7</v>
+      </c>
+      <c r="E163" t="s">
+        <v>29</v>
+      </c>
+      <c r="F163" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164">
+        <v>3541406</v>
+      </c>
+      <c r="D164" t="s">
+        <v>7</v>
+      </c>
+      <c r="E164" t="s">
+        <v>30</v>
+      </c>
+      <c r="F164" s="1">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165" t="s">
+        <v>6</v>
+      </c>
+      <c r="C165">
+        <v>3541406</v>
+      </c>
+      <c r="D165" t="s">
+        <v>7</v>
+      </c>
+      <c r="E165" t="s">
+        <v>31</v>
+      </c>
+      <c r="F165" s="1">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166" t="s">
+        <v>6</v>
+      </c>
+      <c r="C166">
+        <v>3541406</v>
+      </c>
+      <c r="D166" t="s">
+        <v>7</v>
+      </c>
+      <c r="E166" t="s">
+        <v>32</v>
+      </c>
+      <c r="F166" s="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167">
+        <v>3541406</v>
+      </c>
+      <c r="D167" t="s">
+        <v>7</v>
+      </c>
+      <c r="E167" t="s">
+        <v>33</v>
+      </c>
+      <c r="F167" s="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168">
+        <v>3541406</v>
+      </c>
+      <c r="D168" t="s">
+        <v>7</v>
+      </c>
+      <c r="E168" t="s">
+        <v>34</v>
+      </c>
+      <c r="F168" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169">
+        <v>3541406</v>
+      </c>
+      <c r="D169" t="s">
+        <v>7</v>
+      </c>
+      <c r="E169" t="s">
+        <v>35</v>
+      </c>
+      <c r="F169" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>5</v>
+      </c>
+      <c r="B170" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170">
+        <v>3541406</v>
+      </c>
+      <c r="D170" t="s">
+        <v>7</v>
+      </c>
+      <c r="E170" t="s">
+        <v>36</v>
+      </c>
+      <c r="F170" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>5</v>
+      </c>
+      <c r="B171" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171">
+        <v>3541406</v>
+      </c>
+      <c r="D171" t="s">
+        <v>7</v>
+      </c>
+      <c r="E171" t="s">
+        <v>37</v>
+      </c>
+      <c r="F171" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172" t="s">
+        <v>6</v>
+      </c>
+      <c r="C172">
+        <v>3541406</v>
+      </c>
+      <c r="D172" t="s">
+        <v>7</v>
+      </c>
+      <c r="E172" t="s">
+        <v>38</v>
+      </c>
+      <c r="F172" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>5</v>
+      </c>
+      <c r="B173" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173">
+        <v>3541406</v>
+      </c>
+      <c r="D173" t="s">
+        <v>7</v>
+      </c>
+      <c r="E173" t="s">
+        <v>39</v>
+      </c>
+      <c r="F173" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>5</v>
+      </c>
+      <c r="B174" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174">
+        <v>3541406</v>
+      </c>
+      <c r="D174" t="s">
+        <v>7</v>
+      </c>
+      <c r="E174" t="s">
+        <v>40</v>
+      </c>
+      <c r="F174" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>5</v>
+      </c>
+      <c r="B175" t="s">
+        <v>6</v>
+      </c>
+      <c r="C175">
+        <v>3541406</v>
+      </c>
+      <c r="D175" t="s">
+        <v>7</v>
+      </c>
+      <c r="E175" t="s">
+        <v>41</v>
+      </c>
+      <c r="F175" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>5</v>
+      </c>
+      <c r="B176" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176">
+        <v>3541406</v>
+      </c>
+      <c r="D176" t="s">
+        <v>7</v>
+      </c>
+      <c r="E176" t="s">
+        <v>42</v>
+      </c>
+      <c r="F176" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>5</v>
+      </c>
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177">
+        <v>3541406</v>
+      </c>
+      <c r="D177" t="s">
+        <v>7</v>
+      </c>
+      <c r="E177" t="s">
+        <v>43</v>
+      </c>
+      <c r="F177" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>5</v>
+      </c>
+      <c r="B178" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178">
+        <v>3541406</v>
+      </c>
+      <c r="D178" t="s">
+        <v>7</v>
+      </c>
+      <c r="E178" t="s">
+        <v>44</v>
+      </c>
+      <c r="F178" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>5</v>
+      </c>
+      <c r="B179" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179">
+        <v>3541406</v>
+      </c>
+      <c r="D179" t="s">
+        <v>7</v>
+      </c>
+      <c r="E179" t="s">
+        <v>45</v>
+      </c>
+      <c r="F179" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>5</v>
+      </c>
+      <c r="B180" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180">
+        <v>3541406</v>
+      </c>
+      <c r="D180" t="s">
+        <v>7</v>
+      </c>
+      <c r="E180" t="s">
         <v>46</v>
       </c>
-      <c r="F92" s="1">
-        <v>48</v>
+      <c r="F180" s="1">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F92">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F180">
       <sortCondition ref="E1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
chore: update dengue database with data from 2022 to 2027 week 27
</commit_message>
<xml_diff>
--- a/data/bronze/dengue_prudente_weekly.xlsx
+++ b/data/bronze/dengue_prudente_weekly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryann\Documents\Projetos RStudio\dengue-project\data\bronze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE331FB-EBFD-4CDE-94E0-E42C9B391549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4220FF81-AC8B-4228-A4A9-9FA0B851B57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="204">
   <si>
     <t>Região|UF|Município</t>
   </si>
@@ -592,6 +592,54 @@
   </si>
   <si>
     <t>2023/52</t>
+  </si>
+  <si>
+    <t>2022/01</t>
+  </si>
+  <si>
+    <t>2022/02</t>
+  </si>
+  <si>
+    <t>2022/03</t>
+  </si>
+  <si>
+    <t>2022/04</t>
+  </si>
+  <si>
+    <t>2022/05</t>
+  </si>
+  <si>
+    <t>2022/06</t>
+  </si>
+  <si>
+    <t>2022/07</t>
+  </si>
+  <si>
+    <t>2022/08</t>
+  </si>
+  <si>
+    <t>2022/09</t>
+  </si>
+  <si>
+    <t>2022/10</t>
+  </si>
+  <si>
+    <t>2022/11</t>
+  </si>
+  <si>
+    <t>2022/12</t>
+  </si>
+  <si>
+    <t>2022/13</t>
+  </si>
+  <si>
+    <t>2022/14</t>
+  </si>
+  <si>
+    <t>2022/15</t>
+  </si>
+  <si>
+    <t>2022/16</t>
   </si>
 </sst>
 </file>
@@ -644,9 +692,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F180"/>
+  <dimension ref="A1:G196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -977,16 +1026,16 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>3541459</v>
+        <v>3541407</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>188</v>
       </c>
       <c r="F2" s="1">
-        <v>766</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -997,16 +1046,16 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>3541460</v>
+        <v>3541408</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="F3" s="1">
-        <v>926</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1017,16 +1066,16 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>3541461</v>
+        <v>3541409</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>190</v>
       </c>
       <c r="F4" s="1">
-        <v>674</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1037,16 +1086,16 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>3541462</v>
+        <v>3541410</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>191</v>
       </c>
       <c r="F5" s="1">
-        <v>502</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1057,16 +1106,16 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>3541463</v>
+        <v>3541411</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>192</v>
       </c>
       <c r="F6" s="1">
-        <v>434</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1077,16 +1126,16 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>3541464</v>
+        <v>3541412</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>193</v>
       </c>
       <c r="F7" s="1">
-        <v>447</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1097,16 +1146,16 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>3541465</v>
+        <v>3541413</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>194</v>
       </c>
       <c r="F8" s="1">
-        <v>405</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1117,16 +1166,16 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>3541466</v>
+        <v>3541414</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>195</v>
       </c>
       <c r="F9" s="1">
-        <v>288</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1137,16 +1186,16 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>3541467</v>
+        <v>3541415</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>196</v>
       </c>
       <c r="F10" s="1">
-        <v>203</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1157,16 +1206,16 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>3541468</v>
+        <v>3541416</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>197</v>
       </c>
       <c r="F11" s="1">
-        <v>175</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1177,16 +1226,16 @@
         <v>6</v>
       </c>
       <c r="C12">
-        <v>3541469</v>
+        <v>3541417</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>110</v>
+        <v>198</v>
       </c>
       <c r="F12" s="1">
-        <v>140</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1197,16 +1246,16 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>3541470</v>
+        <v>3541418</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>199</v>
       </c>
       <c r="F13" s="1">
-        <v>73</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1217,16 +1266,16 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>3541471</v>
+        <v>3541419</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>112</v>
+        <v>200</v>
       </c>
       <c r="F14" s="1">
-        <v>30</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1237,16 +1286,16 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <v>3541472</v>
+        <v>3541420</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="F15" s="1">
-        <v>35</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1257,16 +1306,16 @@
         <v>6</v>
       </c>
       <c r="C16">
-        <v>3541473</v>
+        <v>3541421</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>202</v>
       </c>
       <c r="F16" s="1">
-        <v>32</v>
+        <v>523</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1277,16 +1326,16 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>3541474</v>
+        <v>3541422</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>203</v>
       </c>
       <c r="F17" s="1">
-        <v>19</v>
+        <v>580</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1297,16 +1346,16 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>3541475</v>
+        <v>3541459</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="F18" s="1">
-        <v>12</v>
+        <v>766</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1317,16 +1366,16 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>3541476</v>
+        <v>3541460</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="F19" s="1">
-        <v>8</v>
+        <v>926</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1337,16 +1386,16 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>3541477</v>
+        <v>3541461</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="F20" s="1">
-        <v>3</v>
+        <v>674</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1357,16 +1406,16 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>3541478</v>
+        <v>3541462</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="F21" s="1">
-        <v>9</v>
+        <v>502</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1377,16 +1426,16 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <v>3541479</v>
+        <v>3541463</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="F22" s="1">
-        <v>6</v>
+        <v>434</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1397,16 +1446,16 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <v>3541480</v>
+        <v>3541464</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="F23" s="1">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1417,16 +1466,16 @@
         <v>6</v>
       </c>
       <c r="C24">
-        <v>3541481</v>
+        <v>3541465</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F24" s="1">
-        <v>5</v>
+        <v>405</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1437,16 +1486,16 @@
         <v>6</v>
       </c>
       <c r="C25">
-        <v>3541482</v>
+        <v>3541466</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="F25" s="1">
-        <v>6</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1457,16 +1506,16 @@
         <v>6</v>
       </c>
       <c r="C26">
-        <v>3541483</v>
+        <v>3541467</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F26" s="1">
-        <v>5</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1477,16 +1526,16 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <v>3541484</v>
+        <v>3541468</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="F27" s="1">
-        <v>5</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1497,16 +1546,16 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>3541485</v>
+        <v>3541469</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="F28" s="1">
-        <v>9</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1517,16 +1566,16 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>3541486</v>
+        <v>3541470</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="F29" s="1">
-        <v>14</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1537,16 +1586,16 @@
         <v>6</v>
       </c>
       <c r="C30">
-        <v>3541487</v>
+        <v>3541471</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="F30" s="1">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1557,16 +1606,16 @@
         <v>6</v>
       </c>
       <c r="C31">
-        <v>3541488</v>
+        <v>3541472</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="F31" s="1">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1577,16 +1626,16 @@
         <v>6</v>
       </c>
       <c r="C32">
-        <v>3541489</v>
+        <v>3541473</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="F32" s="1">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1597,16 +1646,16 @@
         <v>6</v>
       </c>
       <c r="C33">
-        <v>3541490</v>
+        <v>3541474</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="F33" s="1">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1617,16 +1666,16 @@
         <v>6</v>
       </c>
       <c r="C34">
-        <v>3541491</v>
+        <v>3541475</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="F34" s="1">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1637,16 +1686,16 @@
         <v>6</v>
       </c>
       <c r="C35">
-        <v>3541492</v>
+        <v>3541476</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="F35" s="1">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1657,16 +1706,16 @@
         <v>6</v>
       </c>
       <c r="C36">
-        <v>3541493</v>
+        <v>3541477</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="F36" s="1">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1677,16 +1726,16 @@
         <v>6</v>
       </c>
       <c r="C37">
-        <v>3541494</v>
+        <v>3541478</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="F37" s="1">
-        <v>40</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1697,16 +1746,16 @@
         <v>6</v>
       </c>
       <c r="C38">
-        <v>3541407</v>
+        <v>3541479</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="F38" s="1">
-        <v>316</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1717,16 +1766,16 @@
         <v>6</v>
       </c>
       <c r="C39">
-        <v>3541408</v>
+        <v>3541480</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="F39" s="1">
-        <v>357</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1737,16 +1786,16 @@
         <v>6</v>
       </c>
       <c r="C40">
-        <v>3541409</v>
+        <v>3541481</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F40" s="1">
-        <v>410</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1757,16 +1806,16 @@
         <v>6</v>
       </c>
       <c r="C41">
-        <v>3541410</v>
+        <v>3541482</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F41" s="1">
-        <v>601</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1777,16 +1826,16 @@
         <v>6</v>
       </c>
       <c r="C42">
-        <v>3541411</v>
+        <v>3541483</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F42" s="1">
-        <v>782</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1797,16 +1846,16 @@
         <v>6</v>
       </c>
       <c r="C43">
-        <v>3541412</v>
+        <v>3541484</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F43" s="1">
-        <v>1073</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1817,16 +1866,16 @@
         <v>6</v>
       </c>
       <c r="C44">
-        <v>3541413</v>
+        <v>3541485</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="F44" s="1">
-        <v>1485</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1837,16 +1886,16 @@
         <v>6</v>
       </c>
       <c r="C45">
-        <v>3541414</v>
+        <v>3541486</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="F45" s="1">
-        <v>1529</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1857,16 +1906,16 @@
         <v>6</v>
       </c>
       <c r="C46">
-        <v>3541415</v>
+        <v>3541487</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
       </c>
       <c r="E46" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="F46" s="1">
-        <v>2112</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1877,16 +1926,16 @@
         <v>6</v>
       </c>
       <c r="C47">
-        <v>3541416</v>
+        <v>3541488</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="F47" s="1">
-        <v>2757</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1897,16 +1946,16 @@
         <v>6</v>
       </c>
       <c r="C48">
-        <v>3541417</v>
+        <v>3541489</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="F48" s="1">
-        <v>2893</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1917,16 +1966,16 @@
         <v>6</v>
       </c>
       <c r="C49">
-        <v>3541418</v>
+        <v>3541490</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F49" s="1">
-        <v>3321</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1937,16 +1986,16 @@
         <v>6</v>
       </c>
       <c r="C50">
-        <v>3541419</v>
+        <v>3541491</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
       </c>
       <c r="E50" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="F50" s="1">
-        <v>3779</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1957,16 +2006,16 @@
         <v>6</v>
       </c>
       <c r="C51">
-        <v>3541420</v>
+        <v>3541492</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="F51" s="1">
-        <v>3144</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1977,16 +2026,16 @@
         <v>6</v>
       </c>
       <c r="C52">
-        <v>3541421</v>
+        <v>3541493</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
       </c>
       <c r="E52" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="F52" s="1">
-        <v>2966</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1997,16 +2046,16 @@
         <v>6</v>
       </c>
       <c r="C53">
-        <v>3541422</v>
+        <v>3541494</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="F53" s="1">
-        <v>2190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2017,16 +2066,16 @@
         <v>6</v>
       </c>
       <c r="C54">
-        <v>3541423</v>
+        <v>3541407</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="F54" s="1">
-        <v>1562</v>
+        <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2037,16 +2086,16 @@
         <v>6</v>
       </c>
       <c r="C55">
-        <v>3541424</v>
+        <v>3541408</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
       </c>
       <c r="E55" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="F55" s="1">
-        <v>1473</v>
+        <v>357</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2057,16 +2106,16 @@
         <v>6</v>
       </c>
       <c r="C56">
-        <v>3541425</v>
+        <v>3541409</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="F56" s="1">
-        <v>1147</v>
+        <v>410</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2077,16 +2126,16 @@
         <v>6</v>
       </c>
       <c r="C57">
-        <v>3541426</v>
+        <v>3541410</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
       </c>
       <c r="E57" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="F57" s="1">
-        <v>847</v>
+        <v>601</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2097,16 +2146,16 @@
         <v>6</v>
       </c>
       <c r="C58">
-        <v>3541427</v>
+        <v>3541411</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="F58" s="1">
-        <v>471</v>
+        <v>782</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2117,16 +2166,16 @@
         <v>6</v>
       </c>
       <c r="C59">
-        <v>3541428</v>
+        <v>3541412</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="F59" s="1">
-        <v>325</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2137,16 +2186,16 @@
         <v>6</v>
       </c>
       <c r="C60">
-        <v>3541429</v>
+        <v>3541413</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="F60" s="1">
-        <v>194</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2157,16 +2206,16 @@
         <v>6</v>
       </c>
       <c r="C61">
-        <v>3541430</v>
+        <v>3541414</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="F61" s="1">
-        <v>147</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2177,16 +2226,16 @@
         <v>6</v>
       </c>
       <c r="C62">
-        <v>3541431</v>
+        <v>3541415</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="F62" s="1">
-        <v>114</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2197,16 +2246,16 @@
         <v>6</v>
       </c>
       <c r="C63">
-        <v>3541432</v>
+        <v>3541416</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="F63" s="1">
-        <v>58</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2217,16 +2266,16 @@
         <v>6</v>
       </c>
       <c r="C64">
-        <v>3541433</v>
+        <v>3541417</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="F64" s="1">
-        <v>16</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2237,16 +2286,16 @@
         <v>6</v>
       </c>
       <c r="C65">
-        <v>3541434</v>
+        <v>3541418</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F65" s="1">
-        <v>8</v>
+        <v>3321</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2257,16 +2306,16 @@
         <v>6</v>
       </c>
       <c r="C66">
-        <v>3541435</v>
+        <v>3541419</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="F66" s="1">
-        <v>3</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2277,16 +2326,16 @@
         <v>6</v>
       </c>
       <c r="C67">
-        <v>3541436</v>
+        <v>3541420</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
       </c>
       <c r="E67" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="F67" s="1">
-        <v>14</v>
+        <v>3144</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2297,16 +2346,16 @@
         <v>6</v>
       </c>
       <c r="C68">
-        <v>3541437</v>
+        <v>3541421</v>
       </c>
       <c r="D68" t="s">
         <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="F68" s="1">
-        <v>3</v>
+        <v>2966</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2317,16 +2366,16 @@
         <v>6</v>
       </c>
       <c r="C69">
-        <v>3541438</v>
+        <v>3541422</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
       </c>
       <c r="E69" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="F69" s="1">
-        <v>2</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2337,16 +2386,16 @@
         <v>6</v>
       </c>
       <c r="C70">
-        <v>3541439</v>
+        <v>3541423</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="F70" s="1">
-        <v>9</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2357,16 +2406,16 @@
         <v>6</v>
       </c>
       <c r="C71">
-        <v>3541440</v>
+        <v>3541424</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
       </c>
       <c r="E71" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="F71" s="1">
-        <v>3</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2377,16 +2426,16 @@
         <v>6</v>
       </c>
       <c r="C72">
-        <v>3541441</v>
+        <v>3541425</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
       </c>
       <c r="E72" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="F72" s="1">
-        <v>2</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2397,16 +2446,16 @@
         <v>6</v>
       </c>
       <c r="C73">
-        <v>3541442</v>
+        <v>3541426</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
       </c>
       <c r="E73" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="F73" s="1">
-        <v>3</v>
+        <v>847</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2417,16 +2466,16 @@
         <v>6</v>
       </c>
       <c r="C74">
-        <v>3541443</v>
+        <v>3541427</v>
       </c>
       <c r="D74" t="s">
         <v>7</v>
       </c>
       <c r="E74" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="F74" s="1">
-        <v>0</v>
+        <v>471</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2437,16 +2486,16 @@
         <v>6</v>
       </c>
       <c r="C75">
-        <v>3541444</v>
+        <v>3541428</v>
       </c>
       <c r="D75" t="s">
         <v>7</v>
       </c>
       <c r="E75" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="F75" s="1">
-        <v>3</v>
+        <v>325</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2457,16 +2506,16 @@
         <v>6</v>
       </c>
       <c r="C76">
-        <v>3541445</v>
+        <v>3541429</v>
       </c>
       <c r="D76" t="s">
         <v>7</v>
       </c>
       <c r="E76" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="F76" s="1">
-        <v>5</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2477,16 +2526,16 @@
         <v>6</v>
       </c>
       <c r="C77">
-        <v>3541446</v>
+        <v>3541430</v>
       </c>
       <c r="D77" t="s">
         <v>7</v>
       </c>
       <c r="E77" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="F77" s="1">
-        <v>0</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2497,16 +2546,16 @@
         <v>6</v>
       </c>
       <c r="C78">
-        <v>3541447</v>
+        <v>3541431</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
       </c>
       <c r="E78" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="F78" s="1">
-        <v>4</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2517,16 +2566,16 @@
         <v>6</v>
       </c>
       <c r="C79">
-        <v>3541448</v>
+        <v>3541432</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
       </c>
       <c r="E79" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="F79" s="1">
-        <v>4</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2537,16 +2586,16 @@
         <v>6</v>
       </c>
       <c r="C80">
-        <v>3541449</v>
+        <v>3541433</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
       </c>
       <c r="E80" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="F80" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2557,16 +2606,16 @@
         <v>6</v>
       </c>
       <c r="C81">
-        <v>3541450</v>
+        <v>3541434</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
       </c>
       <c r="E81" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="F81" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2577,16 +2626,16 @@
         <v>6</v>
       </c>
       <c r="C82">
-        <v>3541451</v>
+        <v>3541435</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
       </c>
       <c r="E82" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="F82" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2597,16 +2646,16 @@
         <v>6</v>
       </c>
       <c r="C83">
-        <v>3541452</v>
+        <v>3541436</v>
       </c>
       <c r="D83" t="s">
         <v>7</v>
       </c>
       <c r="E83" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="F83" s="1">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2617,16 +2666,16 @@
         <v>6</v>
       </c>
       <c r="C84">
-        <v>3541453</v>
+        <v>3541437</v>
       </c>
       <c r="D84" t="s">
         <v>7</v>
       </c>
       <c r="E84" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="F84" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2637,16 +2686,16 @@
         <v>6</v>
       </c>
       <c r="C85">
-        <v>3541454</v>
+        <v>3541438</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
       </c>
       <c r="E85" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="F85" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2657,16 +2706,16 @@
         <v>6</v>
       </c>
       <c r="C86">
-        <v>3541455</v>
+        <v>3541439</v>
       </c>
       <c r="D86" t="s">
         <v>7</v>
       </c>
       <c r="E86" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="F86" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2677,16 +2726,16 @@
         <v>6</v>
       </c>
       <c r="C87">
-        <v>3541456</v>
+        <v>3541440</v>
       </c>
       <c r="D87" t="s">
         <v>7</v>
       </c>
       <c r="E87" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="F87" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2697,16 +2746,16 @@
         <v>6</v>
       </c>
       <c r="C88">
-        <v>3541457</v>
+        <v>3541441</v>
       </c>
       <c r="D88" t="s">
         <v>7</v>
       </c>
       <c r="E88" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="F88" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2717,16 +2766,16 @@
         <v>6</v>
       </c>
       <c r="C89">
-        <v>3541458</v>
+        <v>3541442</v>
       </c>
       <c r="D89" t="s">
         <v>7</v>
       </c>
       <c r="E89" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="F89" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2737,16 +2786,16 @@
         <v>6</v>
       </c>
       <c r="C90">
-        <v>3541407</v>
+        <v>3541443</v>
       </c>
       <c r="D90" t="s">
         <v>7</v>
       </c>
       <c r="E90" t="s">
-        <v>48</v>
+        <v>172</v>
       </c>
       <c r="F90" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2757,13 +2806,13 @@
         <v>6</v>
       </c>
       <c r="C91">
-        <v>3541408</v>
+        <v>3541444</v>
       </c>
       <c r="D91" t="s">
         <v>7</v>
       </c>
       <c r="E91" t="s">
-        <v>49</v>
+        <v>173</v>
       </c>
       <c r="F91" s="1">
         <v>3</v>
@@ -2777,16 +2826,16 @@
         <v>6</v>
       </c>
       <c r="C92">
-        <v>3541409</v>
+        <v>3541445</v>
       </c>
       <c r="D92" t="s">
         <v>7</v>
       </c>
       <c r="E92" t="s">
-        <v>50</v>
+        <v>174</v>
       </c>
       <c r="F92" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2797,16 +2846,16 @@
         <v>6</v>
       </c>
       <c r="C93">
-        <v>3541410</v>
+        <v>3541446</v>
       </c>
       <c r="D93" t="s">
         <v>7</v>
       </c>
       <c r="E93" t="s">
-        <v>51</v>
+        <v>175</v>
       </c>
       <c r="F93" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2817,16 +2866,16 @@
         <v>6</v>
       </c>
       <c r="C94">
-        <v>3541411</v>
+        <v>3541447</v>
       </c>
       <c r="D94" t="s">
         <v>7</v>
       </c>
       <c r="E94" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="F94" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2837,16 +2886,16 @@
         <v>6</v>
       </c>
       <c r="C95">
-        <v>3541412</v>
+        <v>3541448</v>
       </c>
       <c r="D95" t="s">
         <v>7</v>
       </c>
       <c r="E95" t="s">
-        <v>53</v>
+        <v>177</v>
       </c>
       <c r="F95" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2857,16 +2906,16 @@
         <v>6</v>
       </c>
       <c r="C96">
-        <v>3541413</v>
+        <v>3541449</v>
       </c>
       <c r="D96" t="s">
         <v>7</v>
       </c>
       <c r="E96" t="s">
-        <v>54</v>
+        <v>178</v>
       </c>
       <c r="F96" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2877,16 +2926,16 @@
         <v>6</v>
       </c>
       <c r="C97">
-        <v>3541414</v>
+        <v>3541450</v>
       </c>
       <c r="D97" t="s">
         <v>7</v>
       </c>
       <c r="E97" t="s">
-        <v>55</v>
+        <v>179</v>
       </c>
       <c r="F97" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2897,16 +2946,16 @@
         <v>6</v>
       </c>
       <c r="C98">
-        <v>3541415</v>
+        <v>3541451</v>
       </c>
       <c r="D98" t="s">
         <v>7</v>
       </c>
       <c r="E98" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
       <c r="F98" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2917,16 +2966,16 @@
         <v>6</v>
       </c>
       <c r="C99">
-        <v>3541416</v>
+        <v>3541452</v>
       </c>
       <c r="D99" t="s">
         <v>7</v>
       </c>
       <c r="E99" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="F99" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2937,16 +2986,16 @@
         <v>6</v>
       </c>
       <c r="C100">
-        <v>3541417</v>
+        <v>3541453</v>
       </c>
       <c r="D100" t="s">
         <v>7</v>
       </c>
       <c r="E100" t="s">
-        <v>58</v>
+        <v>182</v>
       </c>
       <c r="F100" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2957,16 +3006,16 @@
         <v>6</v>
       </c>
       <c r="C101">
-        <v>3541418</v>
+        <v>3541454</v>
       </c>
       <c r="D101" t="s">
         <v>7</v>
       </c>
       <c r="E101" t="s">
-        <v>59</v>
+        <v>183</v>
       </c>
       <c r="F101" s="1">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2977,16 +3026,16 @@
         <v>6</v>
       </c>
       <c r="C102">
-        <v>3541419</v>
+        <v>3541455</v>
       </c>
       <c r="D102" t="s">
         <v>7</v>
       </c>
       <c r="E102" t="s">
-        <v>60</v>
+        <v>184</v>
       </c>
       <c r="F102" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2997,16 +3046,16 @@
         <v>6</v>
       </c>
       <c r="C103">
-        <v>3541420</v>
+        <v>3541456</v>
       </c>
       <c r="D103" t="s">
         <v>7</v>
       </c>
       <c r="E103" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="F103" s="1">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3017,16 +3066,16 @@
         <v>6</v>
       </c>
       <c r="C104">
-        <v>3541421</v>
+        <v>3541457</v>
       </c>
       <c r="D104" t="s">
         <v>7</v>
       </c>
       <c r="E104" t="s">
-        <v>62</v>
+        <v>186</v>
       </c>
       <c r="F104" s="1">
-        <v>36</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3037,16 +3086,16 @@
         <v>6</v>
       </c>
       <c r="C105">
-        <v>3541422</v>
+        <v>3541458</v>
       </c>
       <c r="D105" t="s">
         <v>7</v>
       </c>
       <c r="E105" t="s">
-        <v>63</v>
+        <v>187</v>
       </c>
       <c r="F105" s="1">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3057,16 +3106,16 @@
         <v>6</v>
       </c>
       <c r="C106">
-        <v>3541423</v>
+        <v>3541407</v>
       </c>
       <c r="D106" t="s">
         <v>7</v>
       </c>
       <c r="E106" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F106" s="1">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3077,16 +3126,16 @@
         <v>6</v>
       </c>
       <c r="C107">
-        <v>3541424</v>
+        <v>3541408</v>
       </c>
       <c r="D107" t="s">
         <v>7</v>
       </c>
       <c r="E107" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="F107" s="1">
-        <v>73</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3097,16 +3146,16 @@
         <v>6</v>
       </c>
       <c r="C108">
-        <v>3541425</v>
+        <v>3541409</v>
       </c>
       <c r="D108" t="s">
         <v>7</v>
       </c>
       <c r="E108" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F108" s="1">
-        <v>89</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3117,16 +3166,16 @@
         <v>6</v>
       </c>
       <c r="C109">
-        <v>3541426</v>
+        <v>3541410</v>
       </c>
       <c r="D109" t="s">
         <v>7</v>
       </c>
       <c r="E109" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="F109" s="1">
-        <v>106</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3137,16 +3186,16 @@
         <v>6</v>
       </c>
       <c r="C110">
-        <v>3541427</v>
+        <v>3541411</v>
       </c>
       <c r="D110" t="s">
         <v>7</v>
       </c>
       <c r="E110" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="F110" s="1">
-        <v>76</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3157,16 +3206,16 @@
         <v>6</v>
       </c>
       <c r="C111">
-        <v>3541428</v>
+        <v>3541412</v>
       </c>
       <c r="D111" t="s">
         <v>7</v>
       </c>
       <c r="E111" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="F111" s="1">
-        <v>58</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3177,16 +3226,16 @@
         <v>6</v>
       </c>
       <c r="C112">
-        <v>3541429</v>
+        <v>3541413</v>
       </c>
       <c r="D112" t="s">
         <v>7</v>
       </c>
       <c r="E112" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F112" s="1">
-        <v>54</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3197,16 +3246,16 @@
         <v>6</v>
       </c>
       <c r="C113">
-        <v>3541430</v>
+        <v>3541414</v>
       </c>
       <c r="D113" t="s">
         <v>7</v>
       </c>
       <c r="E113" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F113" s="1">
-        <v>56</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3217,16 +3266,16 @@
         <v>6</v>
       </c>
       <c r="C114">
-        <v>3541431</v>
+        <v>3541415</v>
       </c>
       <c r="D114" t="s">
         <v>7</v>
       </c>
       <c r="E114" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F114" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3237,16 +3286,16 @@
         <v>6</v>
       </c>
       <c r="C115">
-        <v>3541432</v>
+        <v>3541416</v>
       </c>
       <c r="D115" t="s">
         <v>7</v>
       </c>
       <c r="E115" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F115" s="1">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3257,16 +3306,16 @@
         <v>6</v>
       </c>
       <c r="C116">
-        <v>3541433</v>
+        <v>3541417</v>
       </c>
       <c r="D116" t="s">
         <v>7</v>
       </c>
       <c r="E116" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F116" s="1">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3277,16 +3326,16 @@
         <v>6</v>
       </c>
       <c r="C117">
-        <v>3541434</v>
+        <v>3541418</v>
       </c>
       <c r="D117" t="s">
         <v>7</v>
       </c>
       <c r="E117" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="F117" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3297,16 +3346,16 @@
         <v>6</v>
       </c>
       <c r="C118">
-        <v>3541435</v>
+        <v>3541419</v>
       </c>
       <c r="D118" t="s">
         <v>7</v>
       </c>
       <c r="E118" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F118" s="1">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3317,16 +3366,16 @@
         <v>6</v>
       </c>
       <c r="C119">
-        <v>3541436</v>
+        <v>3541420</v>
       </c>
       <c r="D119" t="s">
         <v>7</v>
       </c>
       <c r="E119" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="F119" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3337,16 +3386,16 @@
         <v>6</v>
       </c>
       <c r="C120">
-        <v>3541437</v>
+        <v>3541421</v>
       </c>
       <c r="D120" t="s">
         <v>7</v>
       </c>
       <c r="E120" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="F120" s="1">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3357,16 +3406,16 @@
         <v>6</v>
       </c>
       <c r="C121">
-        <v>3541438</v>
+        <v>3541422</v>
       </c>
       <c r="D121" t="s">
         <v>7</v>
       </c>
       <c r="E121" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="F121" s="1">
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3377,16 +3426,16 @@
         <v>6</v>
       </c>
       <c r="C122">
-        <v>3541439</v>
+        <v>3541423</v>
       </c>
       <c r="D122" t="s">
         <v>7</v>
       </c>
       <c r="E122" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="F122" s="1">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3397,16 +3446,16 @@
         <v>6</v>
       </c>
       <c r="C123">
-        <v>3541440</v>
+        <v>3541424</v>
       </c>
       <c r="D123" t="s">
         <v>7</v>
       </c>
       <c r="E123" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F123" s="1">
-        <v>8</v>
+        <v>73</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3417,16 +3466,16 @@
         <v>6</v>
       </c>
       <c r="C124">
-        <v>3541441</v>
+        <v>3541425</v>
       </c>
       <c r="D124" t="s">
         <v>7</v>
       </c>
       <c r="E124" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F124" s="1">
-        <v>6</v>
+        <v>89</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3437,16 +3486,16 @@
         <v>6</v>
       </c>
       <c r="C125">
-        <v>3541442</v>
+        <v>3541426</v>
       </c>
       <c r="D125" t="s">
         <v>7</v>
       </c>
       <c r="E125" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F125" s="1">
-        <v>2</v>
+        <v>106</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3457,16 +3506,16 @@
         <v>6</v>
       </c>
       <c r="C126">
-        <v>3541443</v>
+        <v>3541427</v>
       </c>
       <c r="D126" t="s">
         <v>7</v>
       </c>
       <c r="E126" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F126" s="1">
-        <v>9</v>
+        <v>76</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3477,16 +3526,16 @@
         <v>6</v>
       </c>
       <c r="C127">
-        <v>3541444</v>
+        <v>3541428</v>
       </c>
       <c r="D127" t="s">
         <v>7</v>
       </c>
       <c r="E127" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F127" s="1">
-        <v>6</v>
+        <v>58</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3497,16 +3546,16 @@
         <v>6</v>
       </c>
       <c r="C128">
-        <v>3541445</v>
+        <v>3541429</v>
       </c>
       <c r="D128" t="s">
         <v>7</v>
       </c>
       <c r="E128" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F128" s="1">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3517,16 +3566,16 @@
         <v>6</v>
       </c>
       <c r="C129">
-        <v>3541446</v>
+        <v>3541430</v>
       </c>
       <c r="D129" t="s">
         <v>7</v>
       </c>
       <c r="E129" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="F129" s="1">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3537,16 +3586,16 @@
         <v>6</v>
       </c>
       <c r="C130">
-        <v>3541447</v>
+        <v>3541431</v>
       </c>
       <c r="D130" t="s">
         <v>7</v>
       </c>
       <c r="E130" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F130" s="1">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3557,16 +3606,16 @@
         <v>6</v>
       </c>
       <c r="C131">
-        <v>3541448</v>
+        <v>3541432</v>
       </c>
       <c r="D131" t="s">
         <v>7</v>
       </c>
       <c r="E131" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F131" s="1">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3577,16 +3626,16 @@
         <v>6</v>
       </c>
       <c r="C132">
-        <v>3541449</v>
+        <v>3541433</v>
       </c>
       <c r="D132" t="s">
         <v>7</v>
       </c>
       <c r="E132" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="F132" s="1">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3597,16 +3646,16 @@
         <v>6</v>
       </c>
       <c r="C133">
-        <v>3541450</v>
+        <v>3541434</v>
       </c>
       <c r="D133" t="s">
         <v>7</v>
       </c>
       <c r="E133" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F133" s="1">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3617,16 +3666,16 @@
         <v>6</v>
       </c>
       <c r="C134">
-        <v>3541451</v>
+        <v>3541435</v>
       </c>
       <c r="D134" t="s">
         <v>7</v>
       </c>
       <c r="E134" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F134" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3637,16 +3686,16 @@
         <v>6</v>
       </c>
       <c r="C135">
-        <v>3541452</v>
+        <v>3541436</v>
       </c>
       <c r="D135" t="s">
         <v>7</v>
       </c>
       <c r="E135" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="F135" s="1">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3657,16 +3706,16 @@
         <v>6</v>
       </c>
       <c r="C136">
-        <v>3541453</v>
+        <v>3541437</v>
       </c>
       <c r="D136" t="s">
         <v>7</v>
       </c>
       <c r="E136" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F136" s="1">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3677,13 +3726,13 @@
         <v>6</v>
       </c>
       <c r="C137">
-        <v>3541454</v>
+        <v>3541438</v>
       </c>
       <c r="D137" t="s">
         <v>7</v>
       </c>
       <c r="E137" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F137" s="1">
         <v>13</v>
@@ -3697,16 +3746,16 @@
         <v>6</v>
       </c>
       <c r="C138">
-        <v>3541455</v>
+        <v>3541439</v>
       </c>
       <c r="D138" t="s">
         <v>7</v>
       </c>
       <c r="E138" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="F138" s="1">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3717,16 +3766,16 @@
         <v>6</v>
       </c>
       <c r="C139">
-        <v>3541456</v>
+        <v>3541440</v>
       </c>
       <c r="D139" t="s">
         <v>7</v>
       </c>
       <c r="E139" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="F139" s="1">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3737,16 +3786,16 @@
         <v>6</v>
       </c>
       <c r="C140">
-        <v>3541457</v>
+        <v>3541441</v>
       </c>
       <c r="D140" t="s">
         <v>7</v>
       </c>
       <c r="E140" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="F140" s="1">
-        <v>39</v>
+        <v>6</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3757,16 +3806,16 @@
         <v>6</v>
       </c>
       <c r="C141">
-        <v>3541458</v>
+        <v>3541442</v>
       </c>
       <c r="D141" t="s">
         <v>7</v>
       </c>
       <c r="E141" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="F141" s="1">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3777,16 +3826,16 @@
         <v>6</v>
       </c>
       <c r="C142">
-        <v>3541406</v>
+        <v>3541443</v>
       </c>
       <c r="D142" t="s">
         <v>7</v>
       </c>
       <c r="E142" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="F142" s="1">
-        <v>126</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3797,16 +3846,16 @@
         <v>6</v>
       </c>
       <c r="C143">
-        <v>3541406</v>
+        <v>3541444</v>
       </c>
       <c r="D143" t="s">
         <v>7</v>
       </c>
       <c r="E143" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="F143" s="1">
-        <v>158</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3817,16 +3866,16 @@
         <v>6</v>
       </c>
       <c r="C144">
-        <v>3541406</v>
+        <v>3541445</v>
       </c>
       <c r="D144" t="s">
         <v>7</v>
       </c>
       <c r="E144" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="F144" s="1">
-        <v>301</v>
+        <v>13</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -3837,16 +3886,16 @@
         <v>6</v>
       </c>
       <c r="C145">
-        <v>3541406</v>
+        <v>3541446</v>
       </c>
       <c r="D145" t="s">
         <v>7</v>
       </c>
       <c r="E145" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="F145" s="1">
-        <v>381</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -3857,16 +3906,16 @@
         <v>6</v>
       </c>
       <c r="C146">
-        <v>3541406</v>
+        <v>3541447</v>
       </c>
       <c r="D146" t="s">
         <v>7</v>
       </c>
       <c r="E146" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="F146" s="1">
-        <v>763</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -3877,16 +3926,16 @@
         <v>6</v>
       </c>
       <c r="C147">
-        <v>3541406</v>
+        <v>3541448</v>
       </c>
       <c r="D147" t="s">
         <v>7</v>
       </c>
       <c r="E147" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="F147" s="1">
-        <v>1284</v>
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3897,16 +3946,16 @@
         <v>6</v>
       </c>
       <c r="C148">
-        <v>3541406</v>
+        <v>3541449</v>
       </c>
       <c r="D148" t="s">
         <v>7</v>
       </c>
       <c r="E148" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="F148" s="1">
-        <v>2079</v>
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3917,16 +3966,16 @@
         <v>6</v>
       </c>
       <c r="C149">
-        <v>3541406</v>
+        <v>3541450</v>
       </c>
       <c r="D149" t="s">
         <v>7</v>
       </c>
       <c r="E149" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="F149" s="1">
-        <v>2650</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3937,16 +3986,16 @@
         <v>6</v>
       </c>
       <c r="C150">
-        <v>3541406</v>
+        <v>3541451</v>
       </c>
       <c r="D150" t="s">
         <v>7</v>
       </c>
       <c r="E150" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="F150" s="1">
-        <v>2949</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -3957,16 +4006,16 @@
         <v>6</v>
       </c>
       <c r="C151">
-        <v>3541406</v>
+        <v>3541452</v>
       </c>
       <c r="D151" t="s">
         <v>7</v>
       </c>
       <c r="E151" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="F151" s="1">
-        <v>2696</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3977,16 +4026,16 @@
         <v>6</v>
       </c>
       <c r="C152">
-        <v>3541406</v>
+        <v>3541453</v>
       </c>
       <c r="D152" t="s">
         <v>7</v>
       </c>
       <c r="E152" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="F152" s="1">
-        <v>2588</v>
+        <v>17</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -3997,16 +4046,16 @@
         <v>6</v>
       </c>
       <c r="C153">
-        <v>3541406</v>
+        <v>3541454</v>
       </c>
       <c r="D153" t="s">
         <v>7</v>
       </c>
       <c r="E153" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="F153" s="1">
-        <v>2534</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -4017,16 +4066,16 @@
         <v>6</v>
       </c>
       <c r="C154">
-        <v>3541406</v>
+        <v>3541455</v>
       </c>
       <c r="D154" t="s">
         <v>7</v>
       </c>
       <c r="E154" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="F154" s="1">
-        <v>2052</v>
+        <v>21</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -4037,16 +4086,16 @@
         <v>6</v>
       </c>
       <c r="C155">
-        <v>3541406</v>
+        <v>3541456</v>
       </c>
       <c r="D155" t="s">
         <v>7</v>
       </c>
       <c r="E155" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="F155" s="1">
-        <v>1502</v>
+        <v>40</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -4057,16 +4106,16 @@
         <v>6</v>
       </c>
       <c r="C156">
-        <v>3541406</v>
+        <v>3541457</v>
       </c>
       <c r="D156" t="s">
         <v>7</v>
       </c>
       <c r="E156" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="F156" s="1">
-        <v>1168</v>
+        <v>39</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
@@ -4077,16 +4126,16 @@
         <v>6</v>
       </c>
       <c r="C157">
-        <v>3541406</v>
+        <v>3541458</v>
       </c>
       <c r="D157" t="s">
         <v>7</v>
       </c>
       <c r="E157" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="F157" s="1">
-        <v>821</v>
+        <v>33</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -4103,10 +4152,10 @@
         <v>7</v>
       </c>
       <c r="E158" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F158" s="1">
-        <v>674</v>
+        <v>126</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
@@ -4123,10 +4172,10 @@
         <v>7</v>
       </c>
       <c r="E159" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F159" s="1">
-        <v>533</v>
+        <v>158</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
@@ -4143,10 +4192,10 @@
         <v>7</v>
       </c>
       <c r="E160" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="F160" s="1">
-        <v>492</v>
+        <v>301</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
@@ -4163,10 +4212,10 @@
         <v>7</v>
       </c>
       <c r="E161" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F161" s="1">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
@@ -4183,10 +4232,10 @@
         <v>7</v>
       </c>
       <c r="E162" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F162" s="1">
-        <v>357</v>
+        <v>763</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -4203,10 +4252,10 @@
         <v>7</v>
       </c>
       <c r="E163" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="F163" s="1">
-        <v>275</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
@@ -4223,10 +4272,10 @@
         <v>7</v>
       </c>
       <c r="E164" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F164" s="1">
-        <v>264</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
@@ -4243,10 +4292,10 @@
         <v>7</v>
       </c>
       <c r="E165" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F165" s="1">
-        <v>155</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
@@ -4263,10 +4312,10 @@
         <v>7</v>
       </c>
       <c r="E166" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F166" s="1">
-        <v>117</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
@@ -4283,10 +4332,10 @@
         <v>7</v>
       </c>
       <c r="E167" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="F167" s="1">
-        <v>119</v>
+        <v>2696</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
@@ -4303,10 +4352,10 @@
         <v>7</v>
       </c>
       <c r="E168" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F168" s="1">
-        <v>74</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
@@ -4323,10 +4372,10 @@
         <v>7</v>
       </c>
       <c r="E169" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F169" s="1">
-        <v>96</v>
+        <v>2534</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
@@ -4343,10 +4392,10 @@
         <v>7</v>
       </c>
       <c r="E170" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F170" s="1">
-        <v>98</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
@@ -4363,10 +4412,10 @@
         <v>7</v>
       </c>
       <c r="E171" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F171" s="1">
-        <v>61</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
@@ -4383,10 +4432,10 @@
         <v>7</v>
       </c>
       <c r="E172" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="F172" s="1">
-        <v>59</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
@@ -4403,10 +4452,10 @@
         <v>7</v>
       </c>
       <c r="E173" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F173" s="1">
-        <v>44</v>
+        <v>821</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
@@ -4423,10 +4472,10 @@
         <v>7</v>
       </c>
       <c r="E174" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F174" s="1">
-        <v>71</v>
+        <v>674</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
@@ -4443,10 +4492,10 @@
         <v>7</v>
       </c>
       <c r="E175" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F175" s="1">
-        <v>95</v>
+        <v>533</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
@@ -4463,13 +4512,13 @@
         <v>7</v>
       </c>
       <c r="E176" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F176" s="1">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>5</v>
       </c>
@@ -4483,13 +4532,13 @@
         <v>7</v>
       </c>
       <c r="E177" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F177" s="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>5</v>
       </c>
@@ -4503,13 +4552,13 @@
         <v>7</v>
       </c>
       <c r="E178" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="F178" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>5</v>
       </c>
@@ -4523,13 +4572,13 @@
         <v>7</v>
       </c>
       <c r="E179" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F179" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>5</v>
       </c>
@@ -4543,15 +4592,336 @@
         <v>7</v>
       </c>
       <c r="E180" t="s">
+        <v>30</v>
+      </c>
+      <c r="F180" s="1">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>5</v>
+      </c>
+      <c r="B181" t="s">
+        <v>6</v>
+      </c>
+      <c r="C181">
+        <v>3541406</v>
+      </c>
+      <c r="D181" t="s">
+        <v>7</v>
+      </c>
+      <c r="E181" t="s">
+        <v>31</v>
+      </c>
+      <c r="F181" s="1">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>5</v>
+      </c>
+      <c r="B182" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182">
+        <v>3541406</v>
+      </c>
+      <c r="D182" t="s">
+        <v>7</v>
+      </c>
+      <c r="E182" t="s">
+        <v>32</v>
+      </c>
+      <c r="F182" s="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>5</v>
+      </c>
+      <c r="B183" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183">
+        <v>3541406</v>
+      </c>
+      <c r="D183" t="s">
+        <v>7</v>
+      </c>
+      <c r="E183" t="s">
+        <v>33</v>
+      </c>
+      <c r="F183" s="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>5</v>
+      </c>
+      <c r="B184" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184">
+        <v>3541406</v>
+      </c>
+      <c r="D184" t="s">
+        <v>7</v>
+      </c>
+      <c r="E184" t="s">
+        <v>34</v>
+      </c>
+      <c r="F184" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>5</v>
+      </c>
+      <c r="B185" t="s">
+        <v>6</v>
+      </c>
+      <c r="C185">
+        <v>3541406</v>
+      </c>
+      <c r="D185" t="s">
+        <v>7</v>
+      </c>
+      <c r="E185" t="s">
+        <v>35</v>
+      </c>
+      <c r="F185" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>5</v>
+      </c>
+      <c r="B186" t="s">
+        <v>6</v>
+      </c>
+      <c r="C186">
+        <v>3541406</v>
+      </c>
+      <c r="D186" t="s">
+        <v>7</v>
+      </c>
+      <c r="E186" t="s">
+        <v>36</v>
+      </c>
+      <c r="F186" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>5</v>
+      </c>
+      <c r="B187" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187">
+        <v>3541406</v>
+      </c>
+      <c r="D187" t="s">
+        <v>7</v>
+      </c>
+      <c r="E187" t="s">
+        <v>37</v>
+      </c>
+      <c r="F187" s="1">
+        <v>61</v>
+      </c>
+      <c r="G187" s="2"/>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>5</v>
+      </c>
+      <c r="B188" t="s">
+        <v>6</v>
+      </c>
+      <c r="C188">
+        <v>3541406</v>
+      </c>
+      <c r="D188" t="s">
+        <v>7</v>
+      </c>
+      <c r="E188" t="s">
+        <v>38</v>
+      </c>
+      <c r="F188" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>5</v>
+      </c>
+      <c r="B189" t="s">
+        <v>6</v>
+      </c>
+      <c r="C189">
+        <v>3541406</v>
+      </c>
+      <c r="D189" t="s">
+        <v>7</v>
+      </c>
+      <c r="E189" t="s">
+        <v>39</v>
+      </c>
+      <c r="F189" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>5</v>
+      </c>
+      <c r="B190" t="s">
+        <v>6</v>
+      </c>
+      <c r="C190">
+        <v>3541406</v>
+      </c>
+      <c r="D190" t="s">
+        <v>7</v>
+      </c>
+      <c r="E190" t="s">
+        <v>40</v>
+      </c>
+      <c r="F190" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>5</v>
+      </c>
+      <c r="B191" t="s">
+        <v>6</v>
+      </c>
+      <c r="C191">
+        <v>3541406</v>
+      </c>
+      <c r="D191" t="s">
+        <v>7</v>
+      </c>
+      <c r="E191" t="s">
+        <v>41</v>
+      </c>
+      <c r="F191" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>5</v>
+      </c>
+      <c r="B192" t="s">
+        <v>6</v>
+      </c>
+      <c r="C192">
+        <v>3541406</v>
+      </c>
+      <c r="D192" t="s">
+        <v>7</v>
+      </c>
+      <c r="E192" t="s">
+        <v>42</v>
+      </c>
+      <c r="F192" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>5</v>
+      </c>
+      <c r="B193" t="s">
+        <v>6</v>
+      </c>
+      <c r="C193">
+        <v>3541406</v>
+      </c>
+      <c r="D193" t="s">
+        <v>7</v>
+      </c>
+      <c r="E193" t="s">
+        <v>43</v>
+      </c>
+      <c r="F193" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>5</v>
+      </c>
+      <c r="B194" t="s">
+        <v>6</v>
+      </c>
+      <c r="C194">
+        <v>3541406</v>
+      </c>
+      <c r="D194" t="s">
+        <v>7</v>
+      </c>
+      <c r="E194" t="s">
+        <v>44</v>
+      </c>
+      <c r="F194" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>5</v>
+      </c>
+      <c r="B195" t="s">
+        <v>6</v>
+      </c>
+      <c r="C195">
+        <v>3541406</v>
+      </c>
+      <c r="D195" t="s">
+        <v>7</v>
+      </c>
+      <c r="E195" t="s">
+        <v>45</v>
+      </c>
+      <c r="F195" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>5</v>
+      </c>
+      <c r="B196" t="s">
+        <v>6</v>
+      </c>
+      <c r="C196">
+        <v>3541406</v>
+      </c>
+      <c r="D196" t="s">
+        <v>7</v>
+      </c>
+      <c r="E196" t="s">
         <v>46</v>
       </c>
-      <c r="F180" s="1">
+      <c r="F196" s="1">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F180">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F196">
       <sortCondition ref="E1"/>
     </sortState>
   </autoFilter>

</xml_diff>